<commit_message>
fix minor errors, including with CO2 metadata
</commit_message>
<xml_diff>
--- a/data/sampling/ic_icpms/ic_icmps_data.xlsx
+++ b/data/sampling/ic_icpms/ic_icmps_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/ic_icpms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77474E2-70A8-C04D-8A25-6FEE7E58BEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94EEE67-0036-C148-8267-743F7BC21E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="-20940" windowWidth="20020" windowHeight="20940" xr2:uid="{F39F1C9C-1A4D-424E-9A79-2CB6EBF17461}"/>
+    <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{F39F1C9C-1A4D-424E-9A79-2CB6EBF17461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>